<commit_message>
:children_crossing: Improve usability of map-chart combo
* Remove pointer events for hover circle element
* Add tooltip to map
</commit_message>
<xml_diff>
--- a/data/static/Bhos.xlsx
+++ b/data/static/Bhos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakoblistabarth/git/itc-atlas-website/data/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADA201F-72B7-5741-8770-E9D4396DB0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388D3566-C07B-0B44-9A90-F7A9598FD57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{7BAB83D4-346C-D141-B7C7-CC9782BF7A59}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7BAB83D4-346C-D141-B7C7-CC9782BF7A59}"/>
   </bookViews>
   <sheets>
     <sheet name="countries" sheetId="1" r:id="rId1"/>
@@ -138,9 +138,6 @@
     <t>Transition</t>
   </si>
   <si>
-    <t>Country</t>
-  </si>
-  <si>
     <t>Colombia</t>
   </si>
   <si>
@@ -688,6 +685,9 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>General Focus Country</t>
   </si>
 </sst>
 </file>
@@ -1058,8 +1058,8 @@
   <dimension ref="A1:E252"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D84" sqref="D84"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D167" sqref="D167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1070,19 +1070,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1093,24 +1093,24 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1121,10 +1121,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1135,10 +1135,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1149,10 +1149,10 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1163,10 +1163,10 @@
         <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1177,10 +1177,10 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1191,10 +1191,10 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1205,10 +1205,10 @@
         <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1219,10 +1219,10 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1233,10 +1233,10 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1247,10 +1247,10 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1261,10 +1261,10 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1275,10 +1275,10 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1289,21 +1289,21 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D17" t="s">
         <v>31</v>
@@ -1311,13 +1311,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
       <c r="C18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D18" t="s">
         <v>31</v>
@@ -1325,13 +1325,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D19" t="s">
         <v>31</v>
@@ -1345,24 +1345,24 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1373,10 +1373,10 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1387,10 +1387,10 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1401,10 +1401,10 @@
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1415,10 +1415,10 @@
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1429,10 +1429,10 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1443,10 +1443,10 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D27" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1457,10 +1457,10 @@
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1471,10 +1471,10 @@
         <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D29" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1485,10 +1485,10 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1499,10 +1499,10 @@
         <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D31" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1513,10 +1513,10 @@
         <v>20</v>
       </c>
       <c r="C32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D32" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1527,10 +1527,10 @@
         <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D33" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1541,66 +1541,66 @@
         <v>18</v>
       </c>
       <c r="C34" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D34" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1611,13 +1611,13 @@
         <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1628,13 +1628,13 @@
         <v>25</v>
       </c>
       <c r="C40" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1645,47 +1645,47 @@
         <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" t="s">
         <v>49</v>
       </c>
-      <c r="B43" t="s">
-        <v>50</v>
-      </c>
       <c r="C43" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1696,567 +1696,567 @@
         <v>18</v>
       </c>
       <c r="C44" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B45" t="s">
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C47" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C48" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C49" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C50" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C52" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C53" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B54" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C54" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B55" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C55" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" t="s">
         <v>95</v>
       </c>
-      <c r="B57" t="s">
-        <v>96</v>
-      </c>
       <c r="C57" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E57" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" t="s">
         <v>104</v>
       </c>
-      <c r="B58" t="s">
-        <v>105</v>
-      </c>
       <c r="C58" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" t="s">
         <v>106</v>
       </c>
-      <c r="B59" t="s">
-        <v>107</v>
-      </c>
       <c r="C59" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E59" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" t="s">
         <v>108</v>
       </c>
-      <c r="B60" t="s">
-        <v>109</v>
-      </c>
       <c r="C60" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" t="s">
         <v>110</v>
       </c>
-      <c r="B61" t="s">
-        <v>111</v>
-      </c>
       <c r="C61" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E61" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>111</v>
+      </c>
+      <c r="B62" t="s">
         <v>112</v>
       </c>
-      <c r="B62" t="s">
-        <v>113</v>
-      </c>
       <c r="C62" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E62" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C63" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C64" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>91</v>
+      </c>
+      <c r="B65" t="s">
         <v>92</v>
       </c>
-      <c r="B65" t="s">
-        <v>93</v>
-      </c>
       <c r="C65" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E65" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C66" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C67" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C68" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B69" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C69" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C70" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B71" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C71" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B72" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C72" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C73" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B74" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C74" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75" t="s">
         <v>79</v>
       </c>
-      <c r="B75" t="s">
-        <v>80</v>
-      </c>
       <c r="C75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D75" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>34</v>
+      </c>
+      <c r="B76" t="s">
         <v>35</v>
       </c>
-      <c r="B76" t="s">
-        <v>36</v>
-      </c>
       <c r="C76" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B77" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C77" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>213</v>
+      </c>
+      <c r="B78" t="s">
         <v>214</v>
       </c>
-      <c r="B78" t="s">
-        <v>215</v>
-      </c>
       <c r="C78" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D78" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B79" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C79" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>113</v>
+      </c>
+      <c r="B80" t="s">
         <v>114</v>
       </c>
-      <c r="B80" t="s">
-        <v>115</v>
-      </c>
       <c r="C80" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D80" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B81" t="s">
         <v>2</v>
       </c>
       <c r="C81" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D81" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -2267,10 +2267,10 @@
         <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D82" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -2281,10 +2281,10 @@
         <v>27</v>
       </c>
       <c r="C83" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D83" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -2295,10 +2295,10 @@
         <v>28</v>
       </c>
       <c r="C84" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D84" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -2309,10 +2309,10 @@
         <v>26</v>
       </c>
       <c r="C85" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D85" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -2323,10 +2323,10 @@
         <v>25</v>
       </c>
       <c r="C86" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D86" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -2337,10 +2337,10 @@
         <v>24</v>
       </c>
       <c r="C87" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D87" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -2351,10 +2351,10 @@
         <v>23</v>
       </c>
       <c r="C88" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D88" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -2365,10 +2365,10 @@
         <v>30</v>
       </c>
       <c r="C89" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D89" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -2379,10 +2379,10 @@
         <v>21</v>
       </c>
       <c r="C90" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D90" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -2393,10 +2393,10 @@
         <v>20</v>
       </c>
       <c r="C91" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D91" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2407,10 +2407,10 @@
         <v>19</v>
       </c>
       <c r="C92" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D92" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2421,122 +2421,122 @@
         <v>18</v>
       </c>
       <c r="C93" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D93" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>115</v>
+      </c>
+      <c r="C94" t="s">
+        <v>200</v>
+      </c>
+      <c r="D94" t="s">
+        <v>215</v>
+      </c>
+      <c r="E94" t="s">
         <v>116</v>
-      </c>
-      <c r="C94" t="s">
-        <v>201</v>
-      </c>
-      <c r="D94" t="s">
-        <v>32</v>
-      </c>
-      <c r="E94" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B95" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C95" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D95" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96" t="s">
         <v>120</v>
       </c>
-      <c r="B96" t="s">
-        <v>121</v>
-      </c>
       <c r="C96" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D96" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>121</v>
+      </c>
+      <c r="B97" t="s">
         <v>122</v>
       </c>
-      <c r="B97" t="s">
-        <v>123</v>
-      </c>
       <c r="C97" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D97" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B98" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C98" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D98" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B99" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C99" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D99" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>123</v>
+      </c>
+      <c r="B100" t="s">
         <v>124</v>
       </c>
-      <c r="B100" t="s">
-        <v>125</v>
-      </c>
       <c r="C100" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D100" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>125</v>
+      </c>
+      <c r="B101" t="s">
         <v>126</v>
       </c>
-      <c r="B101" t="s">
-        <v>127</v>
-      </c>
       <c r="C101" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D101" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -2547,13 +2547,13 @@
         <v>28</v>
       </c>
       <c r="C102" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D102" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E102" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -2564,13 +2564,13 @@
         <v>25</v>
       </c>
       <c r="C103" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D103" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E103" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -2581,47 +2581,47 @@
         <v>27</v>
       </c>
       <c r="C104" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D104" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E104" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B105" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C105" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D105" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E105" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>48</v>
+      </c>
+      <c r="B106" t="s">
         <v>49</v>
       </c>
-      <c r="B106" t="s">
-        <v>50</v>
-      </c>
       <c r="C106" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D106" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E106" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -2632,13 +2632,13 @@
         <v>18</v>
       </c>
       <c r="C107" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D107" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E107" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -2649,81 +2649,81 @@
         <v>1</v>
       </c>
       <c r="C108" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E108" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B109" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C109" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D109" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E109" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B110" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C110" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D110" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E110" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B111" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C111" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D111" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E111" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B112" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C112" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D112" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E112" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -2734,64 +2734,64 @@
         <v>20</v>
       </c>
       <c r="C113" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D113" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E113" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B114" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C114" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D114" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E114" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B115" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C115" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D115" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E115" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B116" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C116" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D116" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E116" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -2802,387 +2802,387 @@
         <v>6</v>
       </c>
       <c r="C117" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D117" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E117" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B118" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C118" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D118" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E118" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B119" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C119" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D119" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E119" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B120" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C120" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D120" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E120" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
+        <v>143</v>
+      </c>
+      <c r="B121" t="s">
         <v>144</v>
       </c>
-      <c r="B121" t="s">
-        <v>145</v>
-      </c>
       <c r="C121" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D121" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E121" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B122" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C122" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D122" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E122" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B123" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C123" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D123" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E123" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B124" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C124" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D124" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E124" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B125" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C125" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D125" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E125" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B126" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C126" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D126" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E126" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B127" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C127" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D127" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E127" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>105</v>
+      </c>
+      <c r="B128" t="s">
         <v>106</v>
       </c>
-      <c r="B128" t="s">
-        <v>107</v>
-      </c>
       <c r="C128" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D128" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E128" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B129" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C129" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D129" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E129" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B130" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C130" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D130" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E130" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B131" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C131" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D131" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E131" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B132" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C132" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D132" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E132" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B133" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C133" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D133" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E133" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
+        <v>123</v>
+      </c>
+      <c r="B134" t="s">
         <v>124</v>
       </c>
-      <c r="B134" t="s">
-        <v>125</v>
-      </c>
       <c r="C134" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D134" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E134" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
+        <v>94</v>
+      </c>
+      <c r="B135" t="s">
         <v>95</v>
       </c>
-      <c r="B135" t="s">
-        <v>96</v>
-      </c>
       <c r="C135" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D135" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E135" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
+        <v>125</v>
+      </c>
+      <c r="B136" t="s">
         <v>126</v>
       </c>
-      <c r="B136" t="s">
-        <v>127</v>
-      </c>
       <c r="C136" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D136" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E136" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
+        <v>121</v>
+      </c>
+      <c r="B137" t="s">
         <v>122</v>
       </c>
-      <c r="B137" t="s">
-        <v>123</v>
-      </c>
       <c r="C137" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D137" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E137" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
+        <v>119</v>
+      </c>
+      <c r="B138" t="s">
         <v>120</v>
       </c>
-      <c r="B138" t="s">
-        <v>121</v>
-      </c>
       <c r="C138" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D138" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E138" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
+        <v>111</v>
+      </c>
+      <c r="B139" t="s">
         <v>112</v>
       </c>
-      <c r="B139" t="s">
-        <v>113</v>
-      </c>
       <c r="C139" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D139" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E139" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -3193,47 +3193,47 @@
         <v>23</v>
       </c>
       <c r="C140" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D140" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E140" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
+        <v>107</v>
+      </c>
+      <c r="B141" t="s">
         <v>108</v>
       </c>
-      <c r="B141" t="s">
-        <v>109</v>
-      </c>
       <c r="C141" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D141" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E141" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
+        <v>103</v>
+      </c>
+      <c r="B142" t="s">
         <v>104</v>
       </c>
-      <c r="B142" t="s">
-        <v>105</v>
-      </c>
       <c r="C142" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D142" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E142" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
@@ -3244,98 +3244,98 @@
         <v>22</v>
       </c>
       <c r="C143" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D143" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E143" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B144" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C144" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D144" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E144" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B145" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C145" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D145" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E145" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
+        <v>78</v>
+      </c>
+      <c r="B146" t="s">
         <v>79</v>
       </c>
-      <c r="B146" t="s">
-        <v>80</v>
-      </c>
       <c r="C146" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D146" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E146" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B147" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C147" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D147" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E147" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B148" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C148" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D148" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E148" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -3346,81 +3346,81 @@
         <v>24</v>
       </c>
       <c r="C149" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D149" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E149" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B150" t="s">
         <v>2</v>
       </c>
       <c r="C150" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D150" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E150" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B151" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C151" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D151" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E151" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B152" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C152" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D152" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E152" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B153" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C153" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D153" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E153" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -3431,24 +3431,24 @@
         <v>1</v>
       </c>
       <c r="C154" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D154" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B155" t="s">
         <v>2</v>
       </c>
       <c r="C155" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D155" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
@@ -3459,10 +3459,10 @@
         <v>6</v>
       </c>
       <c r="C156" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D156" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
@@ -3473,10 +3473,10 @@
         <v>5</v>
       </c>
       <c r="C157" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D157" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
@@ -3487,10 +3487,10 @@
         <v>27</v>
       </c>
       <c r="C158" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D158" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
@@ -3501,10 +3501,10 @@
         <v>26</v>
       </c>
       <c r="C159" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D159" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
@@ -3515,10 +3515,10 @@
         <v>25</v>
       </c>
       <c r="C160" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D160" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -3529,10 +3529,10 @@
         <v>24</v>
       </c>
       <c r="C161" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D161" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -3543,10 +3543,10 @@
         <v>23</v>
       </c>
       <c r="C162" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D162" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -3557,10 +3557,10 @@
         <v>30</v>
       </c>
       <c r="C163" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D163" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -3571,10 +3571,10 @@
         <v>21</v>
       </c>
       <c r="C164" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D164" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -3585,122 +3585,122 @@
         <v>18</v>
       </c>
       <c r="C165" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D165" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B166" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C166" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D166" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B167" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C167" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D167" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B168" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C168" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D168" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
+        <v>123</v>
+      </c>
+      <c r="B169" t="s">
         <v>124</v>
       </c>
-      <c r="B169" t="s">
-        <v>125</v>
-      </c>
       <c r="C169" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D169" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
+        <v>125</v>
+      </c>
+      <c r="B170" t="s">
         <v>126</v>
       </c>
-      <c r="B170" t="s">
-        <v>127</v>
-      </c>
       <c r="C170" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D170" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B171" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C171" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D171" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B172" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C172" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D172" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B173" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C173" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D173" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
@@ -3711,24 +3711,24 @@
         <v>22</v>
       </c>
       <c r="C174" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D174" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
+        <v>176</v>
+      </c>
+      <c r="B175" t="s">
         <v>177</v>
       </c>
-      <c r="B175" t="s">
-        <v>178</v>
-      </c>
       <c r="C175" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D175" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
@@ -3739,7 +3739,7 @@
         <v>21</v>
       </c>
       <c r="C176" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D176" t="s">
         <v>31</v>
@@ -3747,13 +3747,13 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B177" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C177" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D177" t="s">
         <v>31</v>
@@ -3761,13 +3761,13 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B178" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C178" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D178" t="s">
         <v>31</v>
@@ -3781,7 +3781,7 @@
         <v>20</v>
       </c>
       <c r="C179" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D179" t="s">
         <v>31</v>
@@ -3789,13 +3789,13 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B180" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C180" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D180" t="s">
         <v>31</v>
@@ -3803,13 +3803,13 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B181" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C181" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D181" t="s">
         <v>31</v>
@@ -3823,7 +3823,7 @@
         <v>19</v>
       </c>
       <c r="C182" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D182" t="s">
         <v>31</v>
@@ -3837,7 +3837,7 @@
         <v>18</v>
       </c>
       <c r="C183" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D183" t="s">
         <v>31</v>
@@ -3845,13 +3845,13 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
+        <v>119</v>
+      </c>
+      <c r="B184" t="s">
         <v>120</v>
       </c>
-      <c r="B184" t="s">
-        <v>121</v>
-      </c>
       <c r="C184" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D184" t="s">
         <v>31</v>
@@ -3859,13 +3859,13 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B185" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C185" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D185" t="s">
         <v>31</v>
@@ -3873,13 +3873,13 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B186" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C186" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D186" t="s">
         <v>31</v>
@@ -3887,13 +3887,13 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B187" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C187" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D187" t="s">
         <v>31</v>
@@ -3901,13 +3901,13 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
+        <v>34</v>
+      </c>
+      <c r="B188" t="s">
         <v>35</v>
       </c>
-      <c r="B188" t="s">
-        <v>36</v>
-      </c>
       <c r="C188" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D188" t="s">
         <v>31</v>
@@ -3915,13 +3915,13 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B189" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C189" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D189" t="s">
         <v>31</v>
@@ -3929,257 +3929,257 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B190" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C190" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D190" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E190" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B191" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C191" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D191" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E191" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B192" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C192" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D192" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E192" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
+        <v>105</v>
+      </c>
+      <c r="B193" t="s">
         <v>106</v>
       </c>
-      <c r="B193" t="s">
-        <v>107</v>
-      </c>
       <c r="C193" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D193" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E193" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B194" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C194" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D194" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E194" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B195" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C195" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D195" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E195" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B196" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C196" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D196" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E196" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B197" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C197" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D197" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E197" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B198" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C198" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D198" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E198" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
+        <v>123</v>
+      </c>
+      <c r="B199" t="s">
         <v>124</v>
       </c>
-      <c r="B199" t="s">
-        <v>125</v>
-      </c>
       <c r="C199" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D199" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E199" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
+        <v>94</v>
+      </c>
+      <c r="B200" t="s">
         <v>95</v>
       </c>
-      <c r="B200" t="s">
-        <v>96</v>
-      </c>
       <c r="C200" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D200" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E200" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
+        <v>125</v>
+      </c>
+      <c r="B201" t="s">
         <v>126</v>
       </c>
-      <c r="B201" t="s">
-        <v>127</v>
-      </c>
       <c r="C201" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D201" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E201" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
+        <v>121</v>
+      </c>
+      <c r="B202" t="s">
         <v>122</v>
       </c>
-      <c r="B202" t="s">
-        <v>123</v>
-      </c>
       <c r="C202" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D202" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E202" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
+        <v>119</v>
+      </c>
+      <c r="B203" t="s">
         <v>120</v>
       </c>
-      <c r="B203" t="s">
-        <v>121</v>
-      </c>
       <c r="C203" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D203" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E203" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
+        <v>111</v>
+      </c>
+      <c r="B204" t="s">
         <v>112</v>
       </c>
-      <c r="B204" t="s">
-        <v>113</v>
-      </c>
       <c r="C204" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D204" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E204" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
@@ -4190,47 +4190,47 @@
         <v>23</v>
       </c>
       <c r="C205" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D205" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E205" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
+        <v>107</v>
+      </c>
+      <c r="B206" t="s">
         <v>108</v>
       </c>
-      <c r="B206" t="s">
-        <v>109</v>
-      </c>
       <c r="C206" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D206" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E206" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
+        <v>103</v>
+      </c>
+      <c r="B207" t="s">
         <v>104</v>
       </c>
-      <c r="B207" t="s">
-        <v>105</v>
-      </c>
       <c r="C207" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D207" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E207" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
@@ -4241,98 +4241,98 @@
         <v>22</v>
       </c>
       <c r="C208" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D208" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E208" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B209" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C209" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D209" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E209" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B210" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C210" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D210" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E210" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
+        <v>78</v>
+      </c>
+      <c r="B211" t="s">
         <v>79</v>
       </c>
-      <c r="B211" t="s">
-        <v>80</v>
-      </c>
       <c r="C211" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D211" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E211" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B212" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C212" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D212" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E212" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B213" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C213" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D213" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E213" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
@@ -4343,149 +4343,149 @@
         <v>24</v>
       </c>
       <c r="C214" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D214" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E214" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B215" t="s">
         <v>2</v>
       </c>
       <c r="C215" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D215" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E215" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B216" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C216" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D216" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E216" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B217" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C217" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D217" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E217" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B218" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C218" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D218" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E218" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B219" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C219" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D219" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E219" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B220" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C220" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D220" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E220" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B221" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C221" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D221" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E221" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B222" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C222" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D222" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E222" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
@@ -4496,224 +4496,224 @@
         <v>6</v>
       </c>
       <c r="C223" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D223" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E223" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B224" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C224" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D224" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E224" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B225" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C225" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D225" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E225" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
+        <v>176</v>
+      </c>
+      <c r="B226" t="s">
         <v>177</v>
       </c>
-      <c r="B226" t="s">
-        <v>178</v>
-      </c>
       <c r="C226" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D226" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E226" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
+        <v>180</v>
+      </c>
+      <c r="B227" t="s">
         <v>181</v>
       </c>
-      <c r="B227" t="s">
-        <v>182</v>
-      </c>
       <c r="C227" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D227" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E227" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B228" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C228" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D228" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E228" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B229" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C229" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D229" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B230" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C230" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D230" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B231" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C231" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D231" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B232" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C232" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D232" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B233" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C233" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D233" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B234" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C234" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D234" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
+        <v>182</v>
+      </c>
+      <c r="B235" t="s">
         <v>183</v>
       </c>
-      <c r="B235" t="s">
-        <v>184</v>
-      </c>
       <c r="C235" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D235" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
+        <v>184</v>
+      </c>
+      <c r="B236" t="s">
         <v>185</v>
       </c>
-      <c r="B236" t="s">
-        <v>186</v>
-      </c>
       <c r="C236" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D236" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B237" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C237" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D237" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
@@ -4724,206 +4724,206 @@
         <v>19</v>
       </c>
       <c r="C238" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D238" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B239" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C239" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D239" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B240" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C240" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D240" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B241" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C241" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D241" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
+        <v>103</v>
+      </c>
+      <c r="B242" t="s">
         <v>104</v>
       </c>
-      <c r="B242" t="s">
-        <v>105</v>
-      </c>
       <c r="C242" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D242" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B243" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C243" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D243" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
+        <v>187</v>
+      </c>
+      <c r="B244" t="s">
         <v>188</v>
       </c>
-      <c r="B244" t="s">
-        <v>189</v>
-      </c>
       <c r="C244" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D244" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B245" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C245" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D245" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B246" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C246" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D246" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
+        <v>34</v>
+      </c>
+      <c r="B247" t="s">
         <v>35</v>
       </c>
-      <c r="B247" t="s">
-        <v>36</v>
-      </c>
       <c r="C247" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D247" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B248" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C248" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D248" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
+        <v>213</v>
+      </c>
+      <c r="B249" t="s">
         <v>214</v>
       </c>
-      <c r="B249" t="s">
-        <v>215</v>
-      </c>
       <c r="C249" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D249" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
+        <v>113</v>
+      </c>
+      <c r="B250" t="s">
         <v>114</v>
       </c>
-      <c r="B250" t="s">
-        <v>115</v>
-      </c>
       <c r="C250" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D250" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
+        <v>190</v>
+      </c>
+      <c r="B251" t="s">
         <v>191</v>
       </c>
-      <c r="B251" t="s">
-        <v>192</v>
-      </c>
       <c r="C251" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D251" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
+        <v>192</v>
+      </c>
+      <c r="B252" t="s">
         <v>193</v>
       </c>
-      <c r="B252" t="s">
-        <v>194</v>
-      </c>
       <c r="C252" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D252" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -4949,24 +4949,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" t="s">
         <v>196</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>197</v>
-      </c>
-      <c r="D1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C2" s="2">
         <v>40465</v>
@@ -4977,10 +4977,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C3" s="2">
         <v>41218</v>
@@ -4991,10 +4991,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C4" s="2">
         <v>43034</v>
@@ -5005,10 +5005,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C5" s="2">
         <v>44571</v>
@@ -5020,6 +5020,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="36475ac5-abd1-4075-8c59-d359717e1992">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9eed236c-863e-4468-81ea-a1a5634b1ca6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008DD1877411468B4F8815EFA5DFB25A11" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9a125b572fd0fad8ac03e78f4a292300">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="36475ac5-abd1-4075-8c59-d359717e1992" xmlns:ns3="9eed236c-863e-4468-81ea-a1a5634b1ca6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd01341749c4a99db14a5a7b3c803e50" ns2:_="" ns3:_="">
     <xsd:import namespace="36475ac5-abd1-4075-8c59-d359717e1992"/>
@@ -5256,27 +5276,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45321A69-3AF3-45A5-BA17-9E1CAB2F6123}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9eed236c-863e-4468-81ea-a1a5634b1ca6"/>
+    <ds:schemaRef ds:uri="36475ac5-abd1-4075-8c59-d359717e1992"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="36475ac5-abd1-4075-8c59-d359717e1992">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9eed236c-863e-4468-81ea-a1a5634b1ca6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A499CA7-670F-4DBE-BC8E-D5862FDEEBC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8A2AF83-1D54-4DDE-A325-9B57C637107E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5293,29 +5318,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A499CA7-670F-4DBE-BC8E-D5862FDEEBC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45321A69-3AF3-45A5-BA17-9E1CAB2F6123}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9eed236c-863e-4468-81ea-a1a5634b1ca6"/>
-    <ds:schemaRef ds:uri="36475ac5-abd1-4075-8c59-d359717e1992"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
:card_file_box: Fix typo in cabinet assignment
</commit_message>
<xml_diff>
--- a/data/static/Bhos.xlsx
+++ b/data/static/Bhos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universiteittwente.sharepoint.com/sites/ITCAtlasProject/Gedeelde documenten/Data/Government Policies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakoblistabarth/git/itc-atlas/data/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{EC43B4E0-AC5D-7947-95B9-0D2B5CE599D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A323DBB7-3222-0446-AFCF-A2AA456F6F9A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532FC26F-B626-844F-ADAF-6056CCBDC058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{7BAB83D4-346C-D141-B7C7-CC9782BF7A59}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{7BAB83D4-346C-D141-B7C7-CC9782BF7A59}"/>
   </bookViews>
   <sheets>
     <sheet name="countries" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="300">
   <si>
     <t>countryName</t>
   </si>
@@ -835,9 +835,6 @@
     <t>Koenders</t>
   </si>
   <si>
-    <t>Balkenede IV</t>
-  </si>
-  <si>
     <t>Albania</t>
   </si>
   <si>
@@ -932,6 +929,18 @@
   </si>
   <si>
     <t>General Focus Country</t>
+  </si>
+  <si>
+    <t>Balkenende I</t>
+  </si>
+  <si>
+    <t>Balkenende II</t>
+  </si>
+  <si>
+    <t>Balkenende III</t>
+  </si>
+  <si>
+    <t>Balkenende IV</t>
   </si>
 </sst>
 </file>
@@ -1311,8 +1320,8 @@
   <dimension ref="A1:F541"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A390" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C255" sqref="C255:C290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1340,7 +1349,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1351,10 +1360,10 @@
         <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F2" t="s">
         <v>219</v>
@@ -1368,10 +1377,10 @@
         <v>215</v>
       </c>
       <c r="C3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1382,10 +1391,10 @@
         <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1396,10 +1405,10 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1410,10 +1419,10 @@
         <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1424,10 +1433,10 @@
         <v>216</v>
       </c>
       <c r="C7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1438,10 +1447,10 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1452,10 +1461,10 @@
         <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1466,10 +1475,10 @@
         <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1480,10 +1489,10 @@
         <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1494,10 +1503,10 @@
         <v>218</v>
       </c>
       <c r="C12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1508,10 +1517,10 @@
         <v>217</v>
       </c>
       <c r="C13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1522,10 +1531,10 @@
         <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1539,7 +1548,7 @@
         <v>229</v>
       </c>
       <c r="D15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F15" t="s">
         <v>230</v>
@@ -1556,7 +1565,7 @@
         <v>229</v>
       </c>
       <c r="D16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1570,7 +1579,7 @@
         <v>229</v>
       </c>
       <c r="D17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1584,7 +1593,7 @@
         <v>229</v>
       </c>
       <c r="D18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1598,7 +1607,7 @@
         <v>229</v>
       </c>
       <c r="D19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1612,7 +1621,7 @@
         <v>229</v>
       </c>
       <c r="D20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1626,7 +1635,7 @@
         <v>229</v>
       </c>
       <c r="D21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1640,7 +1649,7 @@
         <v>229</v>
       </c>
       <c r="D22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1654,7 +1663,7 @@
         <v>229</v>
       </c>
       <c r="D23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1668,7 +1677,7 @@
         <v>229</v>
       </c>
       <c r="D24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1682,7 +1691,7 @@
         <v>229</v>
       </c>
       <c r="D25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1696,7 +1705,7 @@
         <v>229</v>
       </c>
       <c r="D26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1710,7 +1719,7 @@
         <v>229</v>
       </c>
       <c r="D27" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1724,7 +1733,7 @@
         <v>229</v>
       </c>
       <c r="D28" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1738,7 +1747,7 @@
         <v>229</v>
       </c>
       <c r="D29" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1752,7 +1761,7 @@
         <v>229</v>
       </c>
       <c r="D30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1766,7 +1775,7 @@
         <v>229</v>
       </c>
       <c r="D31" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1780,7 +1789,7 @@
         <v>229</v>
       </c>
       <c r="D32" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1794,7 +1803,7 @@
         <v>229</v>
       </c>
       <c r="D33" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1805,10 +1814,10 @@
         <v>96</v>
       </c>
       <c r="C34" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F34" t="s">
         <v>231</v>
@@ -1822,10 +1831,10 @@
         <v>215</v>
       </c>
       <c r="C35" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D35" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1836,10 +1845,10 @@
         <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D36" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1850,10 +1859,10 @@
         <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D37" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1864,10 +1873,10 @@
         <v>221</v>
       </c>
       <c r="C38" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D38" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1878,10 +1887,10 @@
         <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D39" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1892,10 +1901,10 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D40" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1906,10 +1915,10 @@
         <v>141</v>
       </c>
       <c r="C41" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D41" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1920,10 +1929,10 @@
         <v>27</v>
       </c>
       <c r="C42" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D42" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1934,10 +1943,10 @@
         <v>223</v>
       </c>
       <c r="C43" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D43" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1948,10 +1957,10 @@
         <v>37</v>
       </c>
       <c r="C44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1962,10 +1971,10 @@
         <v>176</v>
       </c>
       <c r="C45" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D45" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1976,10 +1985,10 @@
         <v>23</v>
       </c>
       <c r="C46" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D46" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -1993,7 +2002,7 @@
         <v>232</v>
       </c>
       <c r="D47" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F47" t="s">
         <v>233</v>
@@ -2010,7 +2019,7 @@
         <v>232</v>
       </c>
       <c r="D48" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -2024,7 +2033,7 @@
         <v>232</v>
       </c>
       <c r="D49" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -2038,7 +2047,7 @@
         <v>232</v>
       </c>
       <c r="D50" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -2052,7 +2061,7 @@
         <v>232</v>
       </c>
       <c r="D51" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -2066,7 +2075,7 @@
         <v>232</v>
       </c>
       <c r="D52" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -2080,7 +2089,7 @@
         <v>232</v>
       </c>
       <c r="D53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -2094,7 +2103,7 @@
         <v>232</v>
       </c>
       <c r="D54" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2108,7 +2117,7 @@
         <v>232</v>
       </c>
       <c r="D55" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -2122,7 +2131,7 @@
         <v>232</v>
       </c>
       <c r="D56" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -2133,10 +2142,10 @@
         <v>96</v>
       </c>
       <c r="C57" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D57" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F57" t="s">
         <v>230</v>
@@ -2150,10 +2159,10 @@
         <v>215</v>
       </c>
       <c r="C58" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D58" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -2164,10 +2173,10 @@
         <v>29</v>
       </c>
       <c r="C59" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D59" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -2178,10 +2187,10 @@
         <v>221</v>
       </c>
       <c r="C60" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D60" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2192,10 +2201,10 @@
         <v>237</v>
       </c>
       <c r="C61" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D61" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -2206,10 +2215,10 @@
         <v>238</v>
       </c>
       <c r="C62" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D62" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -2220,10 +2229,10 @@
         <v>35</v>
       </c>
       <c r="C63" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D63" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -2234,10 +2243,10 @@
         <v>60</v>
       </c>
       <c r="C64" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D64" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -2248,10 +2257,10 @@
         <v>141</v>
       </c>
       <c r="C65" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D65" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2262,10 +2271,10 @@
         <v>15</v>
       </c>
       <c r="C66" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D66" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2276,10 +2285,10 @@
         <v>223</v>
       </c>
       <c r="C67" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D67" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2290,10 +2299,10 @@
         <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D68" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2304,10 +2313,10 @@
         <v>31</v>
       </c>
       <c r="C69" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D69" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2318,10 +2327,10 @@
         <v>11</v>
       </c>
       <c r="C70" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D70" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2332,10 +2341,10 @@
         <v>13</v>
       </c>
       <c r="C71" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D71" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2346,10 +2355,10 @@
         <v>161</v>
       </c>
       <c r="C72" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D72" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2360,10 +2369,10 @@
         <v>143</v>
       </c>
       <c r="C73" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D73" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2374,10 +2383,10 @@
         <v>239</v>
       </c>
       <c r="C74" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D74" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2388,10 +2397,10 @@
         <v>151</v>
       </c>
       <c r="C75" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D75" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2402,10 +2411,10 @@
         <v>157</v>
       </c>
       <c r="C76" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D76" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2416,10 +2425,10 @@
         <v>217</v>
       </c>
       <c r="C77" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D77" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2430,10 +2439,10 @@
         <v>227</v>
       </c>
       <c r="C78" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D78" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2444,10 +2453,10 @@
         <v>245</v>
       </c>
       <c r="C79" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D79" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2458,10 +2467,10 @@
         <v>47</v>
       </c>
       <c r="C80" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D80" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -2472,10 +2481,10 @@
         <v>52</v>
       </c>
       <c r="C81" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D81" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -2486,10 +2495,10 @@
         <v>246</v>
       </c>
       <c r="C82" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D82" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -2500,10 +2509,10 @@
         <v>54</v>
       </c>
       <c r="C83" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D83" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -2514,10 +2523,10 @@
         <v>249</v>
       </c>
       <c r="C84" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D84" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -2528,10 +2537,10 @@
         <v>50</v>
       </c>
       <c r="C85" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D85" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -2542,10 +2551,10 @@
         <v>248</v>
       </c>
       <c r="C86" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D86" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -2553,10 +2562,10 @@
         <v>252</v>
       </c>
       <c r="C87" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D87" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -2567,10 +2576,10 @@
         <v>247</v>
       </c>
       <c r="C88" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D88" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -2581,10 +2590,10 @@
         <v>176</v>
       </c>
       <c r="C89" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D89" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -2595,10 +2604,10 @@
         <v>23</v>
       </c>
       <c r="C90" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D90" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -2609,10 +2618,10 @@
         <v>96</v>
       </c>
       <c r="C91" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D91" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F91" t="s">
         <v>230</v>
@@ -2626,10 +2635,10 @@
         <v>215</v>
       </c>
       <c r="C92" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D92" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -2640,10 +2649,10 @@
         <v>29</v>
       </c>
       <c r="C93" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D93" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -2654,10 +2663,10 @@
         <v>221</v>
       </c>
       <c r="C94" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D94" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -2668,10 +2677,10 @@
         <v>237</v>
       </c>
       <c r="C95" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D95" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -2682,10 +2691,10 @@
         <v>238</v>
       </c>
       <c r="C96" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D96" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -2696,10 +2705,10 @@
         <v>35</v>
       </c>
       <c r="C97" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D97" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -2710,10 +2719,10 @@
         <v>60</v>
       </c>
       <c r="C98" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D98" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -2724,10 +2733,10 @@
         <v>141</v>
       </c>
       <c r="C99" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D99" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -2738,10 +2747,10 @@
         <v>15</v>
       </c>
       <c r="C100" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D100" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -2752,10 +2761,10 @@
         <v>223</v>
       </c>
       <c r="C101" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D101" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -2766,10 +2775,10 @@
         <v>9</v>
       </c>
       <c r="C102" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D102" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -2780,10 +2789,10 @@
         <v>31</v>
       </c>
       <c r="C103" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D103" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -2794,10 +2803,10 @@
         <v>11</v>
       </c>
       <c r="C104" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D104" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -2808,10 +2817,10 @@
         <v>13</v>
       </c>
       <c r="C105" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D105" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -2822,10 +2831,10 @@
         <v>161</v>
       </c>
       <c r="C106" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D106" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -2836,10 +2845,10 @@
         <v>143</v>
       </c>
       <c r="C107" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D107" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -2850,10 +2859,10 @@
         <v>239</v>
       </c>
       <c r="C108" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D108" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -2864,10 +2873,10 @@
         <v>151</v>
       </c>
       <c r="C109" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D109" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -2878,10 +2887,10 @@
         <v>157</v>
       </c>
       <c r="C110" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D110" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -2892,10 +2901,10 @@
         <v>217</v>
       </c>
       <c r="C111" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D111" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -2906,10 +2915,10 @@
         <v>227</v>
       </c>
       <c r="C112" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D112" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -2920,10 +2929,10 @@
         <v>245</v>
       </c>
       <c r="C113" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D113" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -2934,10 +2943,10 @@
         <v>47</v>
       </c>
       <c r="C114" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D114" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -2948,10 +2957,10 @@
         <v>52</v>
       </c>
       <c r="C115" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D115" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -2962,10 +2971,10 @@
         <v>246</v>
       </c>
       <c r="C116" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D116" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -2976,10 +2985,10 @@
         <v>54</v>
       </c>
       <c r="C117" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D117" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -2990,10 +2999,10 @@
         <v>249</v>
       </c>
       <c r="C118" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D118" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -3004,10 +3013,10 @@
         <v>50</v>
       </c>
       <c r="C119" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D119" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -3018,10 +3027,10 @@
         <v>248</v>
       </c>
       <c r="C120" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D120" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -3029,10 +3038,10 @@
         <v>252</v>
       </c>
       <c r="C121" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D121" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -3043,10 +3052,10 @@
         <v>247</v>
       </c>
       <c r="C122" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D122" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -3057,10 +3066,10 @@
         <v>176</v>
       </c>
       <c r="C123" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D123" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
@@ -3071,10 +3080,10 @@
         <v>23</v>
       </c>
       <c r="C124" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D124" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
@@ -3088,7 +3097,7 @@
         <v>250</v>
       </c>
       <c r="D125" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F125" t="s">
         <v>251</v>
@@ -3105,7 +3114,7 @@
         <v>250</v>
       </c>
       <c r="D126" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
@@ -3119,7 +3128,7 @@
         <v>250</v>
       </c>
       <c r="D127" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
@@ -3133,7 +3142,7 @@
         <v>250</v>
       </c>
       <c r="D128" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -3147,7 +3156,7 @@
         <v>250</v>
       </c>
       <c r="D129" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -3161,7 +3170,7 @@
         <v>250</v>
       </c>
       <c r="D130" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -3175,7 +3184,7 @@
         <v>250</v>
       </c>
       <c r="D131" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
@@ -3189,7 +3198,7 @@
         <v>250</v>
       </c>
       <c r="D132" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -3203,7 +3212,7 @@
         <v>250</v>
       </c>
       <c r="D133" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -3217,7 +3226,7 @@
         <v>250</v>
       </c>
       <c r="D134" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -3231,7 +3240,7 @@
         <v>250</v>
       </c>
       <c r="D135" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -3245,7 +3254,7 @@
         <v>250</v>
       </c>
       <c r="D136" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
@@ -3259,7 +3268,7 @@
         <v>250</v>
       </c>
       <c r="D137" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
@@ -3273,7 +3282,7 @@
         <v>250</v>
       </c>
       <c r="D138" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
@@ -3287,7 +3296,7 @@
         <v>250</v>
       </c>
       <c r="D139" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
@@ -3301,7 +3310,7 @@
         <v>250</v>
       </c>
       <c r="D140" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
@@ -3315,7 +3324,7 @@
         <v>250</v>
       </c>
       <c r="D141" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
@@ -3329,7 +3338,7 @@
         <v>250</v>
       </c>
       <c r="D142" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
@@ -3343,7 +3352,7 @@
         <v>250</v>
       </c>
       <c r="D143" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -3357,7 +3366,7 @@
         <v>250</v>
       </c>
       <c r="D144" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
@@ -3371,7 +3380,7 @@
         <v>250</v>
       </c>
       <c r="D145" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
@@ -3385,7 +3394,7 @@
         <v>250</v>
       </c>
       <c r="D146" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
@@ -3396,10 +3405,10 @@
         <v>29</v>
       </c>
       <c r="C147" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D147" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F147" t="s">
         <v>255</v>
@@ -3413,10 +3422,10 @@
         <v>221</v>
       </c>
       <c r="C148" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D148" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
@@ -3427,10 +3436,10 @@
         <v>33</v>
       </c>
       <c r="C149" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D149" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
@@ -3441,10 +3450,10 @@
         <v>40</v>
       </c>
       <c r="C150" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D150" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
@@ -3455,10 +3464,10 @@
         <v>170</v>
       </c>
       <c r="C151" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D151" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
@@ -3469,10 +3478,10 @@
         <v>178</v>
       </c>
       <c r="C152" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D152" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
@@ -3483,10 +3492,10 @@
         <v>257</v>
       </c>
       <c r="C153" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D153" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
@@ -3497,10 +3506,10 @@
         <v>35</v>
       </c>
       <c r="C154" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D154" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
@@ -3511,10 +3520,10 @@
         <v>60</v>
       </c>
       <c r="C155" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D155" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
@@ -3525,10 +3534,10 @@
         <v>141</v>
       </c>
       <c r="C156" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D156" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
@@ -3539,10 +3548,10 @@
         <v>15</v>
       </c>
       <c r="C157" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D157" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
@@ -3553,10 +3562,10 @@
         <v>223</v>
       </c>
       <c r="C158" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D158" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
@@ -3567,10 +3576,10 @@
         <v>9</v>
       </c>
       <c r="C159" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D159" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
@@ -3581,10 +3590,10 @@
         <v>31</v>
       </c>
       <c r="C160" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D160" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -3595,10 +3604,10 @@
         <v>11</v>
       </c>
       <c r="C161" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D161" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -3609,10 +3618,10 @@
         <v>13</v>
       </c>
       <c r="C162" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D162" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -3623,10 +3632,10 @@
         <v>6</v>
       </c>
       <c r="C163" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D163" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -3637,10 +3646,10 @@
         <v>63</v>
       </c>
       <c r="C164" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D164" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -3651,10 +3660,10 @@
         <v>17</v>
       </c>
       <c r="C165" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D165" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -3665,10 +3674,10 @@
         <v>42</v>
       </c>
       <c r="C166" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D166" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
@@ -3679,10 +3688,10 @@
         <v>143</v>
       </c>
       <c r="C167" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D167" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
@@ -3693,10 +3702,10 @@
         <v>161</v>
       </c>
       <c r="C168" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D168" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
@@ -3707,10 +3716,10 @@
         <v>245</v>
       </c>
       <c r="C169" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D169" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
@@ -3721,10 +3730,10 @@
         <v>47</v>
       </c>
       <c r="C170" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D170" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
@@ -3735,10 +3744,10 @@
         <v>52</v>
       </c>
       <c r="C171" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D171" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
@@ -3749,10 +3758,10 @@
         <v>246</v>
       </c>
       <c r="C172" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D172" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
@@ -3763,10 +3772,10 @@
         <v>37</v>
       </c>
       <c r="C173" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D173" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
@@ -3777,10 +3786,10 @@
         <v>176</v>
       </c>
       <c r="C174" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D174" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
@@ -3791,10 +3800,10 @@
         <v>23</v>
       </c>
       <c r="C175" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D175" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
@@ -3805,10 +3814,10 @@
         <v>19</v>
       </c>
       <c r="C176" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D176" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
@@ -3819,10 +3828,10 @@
         <v>215</v>
       </c>
       <c r="C177" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D177" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
@@ -3833,10 +3842,10 @@
         <v>25</v>
       </c>
       <c r="C178" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D178" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
@@ -3847,10 +3856,10 @@
         <v>254</v>
       </c>
       <c r="C179" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D179" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
@@ -3861,24 +3870,24 @@
         <v>261</v>
       </c>
       <c r="C180" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D180" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B181" t="s">
         <v>262</v>
       </c>
       <c r="C181" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D181" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
@@ -3889,10 +3898,10 @@
         <v>260</v>
       </c>
       <c r="C182" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D182" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
@@ -3903,10 +3912,10 @@
         <v>29</v>
       </c>
       <c r="C183" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D183" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F183" t="s">
         <v>255</v>
@@ -3920,10 +3929,10 @@
         <v>221</v>
       </c>
       <c r="C184" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D184" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
@@ -3934,10 +3943,10 @@
         <v>33</v>
       </c>
       <c r="C185" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D185" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
@@ -3948,10 +3957,10 @@
         <v>40</v>
       </c>
       <c r="C186" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D186" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
@@ -3962,10 +3971,10 @@
         <v>170</v>
       </c>
       <c r="C187" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D187" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
@@ -3976,10 +3985,10 @@
         <v>178</v>
       </c>
       <c r="C188" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D188" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
@@ -3990,10 +3999,10 @@
         <v>257</v>
       </c>
       <c r="C189" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D189" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
@@ -4004,10 +4013,10 @@
         <v>35</v>
       </c>
       <c r="C190" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D190" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
@@ -4018,10 +4027,10 @@
         <v>60</v>
       </c>
       <c r="C191" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D191" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
@@ -4032,10 +4041,10 @@
         <v>141</v>
       </c>
       <c r="C192" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D192" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
@@ -4046,10 +4055,10 @@
         <v>15</v>
       </c>
       <c r="C193" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D193" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
@@ -4060,10 +4069,10 @@
         <v>223</v>
       </c>
       <c r="C194" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D194" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
@@ -4074,10 +4083,10 @@
         <v>9</v>
       </c>
       <c r="C195" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D195" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
@@ -4088,10 +4097,10 @@
         <v>31</v>
       </c>
       <c r="C196" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D196" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
@@ -4102,10 +4111,10 @@
         <v>11</v>
       </c>
       <c r="C197" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D197" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
@@ -4116,10 +4125,10 @@
         <v>13</v>
       </c>
       <c r="C198" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D198" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
@@ -4130,10 +4139,10 @@
         <v>6</v>
       </c>
       <c r="C199" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D199" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
@@ -4144,10 +4153,10 @@
         <v>63</v>
       </c>
       <c r="C200" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D200" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
@@ -4158,10 +4167,10 @@
         <v>17</v>
       </c>
       <c r="C201" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D201" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
@@ -4172,10 +4181,10 @@
         <v>42</v>
       </c>
       <c r="C202" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D202" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
@@ -4186,10 +4195,10 @@
         <v>143</v>
       </c>
       <c r="C203" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D203" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
@@ -4200,10 +4209,10 @@
         <v>161</v>
       </c>
       <c r="C204" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D204" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
@@ -4214,10 +4223,10 @@
         <v>245</v>
       </c>
       <c r="C205" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D205" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
@@ -4228,10 +4237,10 @@
         <v>47</v>
       </c>
       <c r="C206" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D206" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
@@ -4242,10 +4251,10 @@
         <v>52</v>
       </c>
       <c r="C207" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D207" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
@@ -4256,10 +4265,10 @@
         <v>246</v>
       </c>
       <c r="C208" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D208" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.2">
@@ -4270,10 +4279,10 @@
         <v>37</v>
       </c>
       <c r="C209" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D209" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
@@ -4284,10 +4293,10 @@
         <v>176</v>
       </c>
       <c r="C210" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D210" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
@@ -4298,10 +4307,10 @@
         <v>23</v>
       </c>
       <c r="C211" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D211" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
@@ -4312,10 +4321,10 @@
         <v>19</v>
       </c>
       <c r="C212" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D212" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
@@ -4326,10 +4335,10 @@
         <v>215</v>
       </c>
       <c r="C213" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D213" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
@@ -4340,10 +4349,10 @@
         <v>25</v>
       </c>
       <c r="C214" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D214" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
@@ -4354,10 +4363,10 @@
         <v>254</v>
       </c>
       <c r="C215" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D215" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
@@ -4368,24 +4377,24 @@
         <v>261</v>
       </c>
       <c r="C216" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D216" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B217" t="s">
         <v>262</v>
       </c>
       <c r="C217" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D217" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
@@ -4396,10 +4405,10 @@
         <v>260</v>
       </c>
       <c r="C218" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D218" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
@@ -4410,10 +4419,10 @@
         <v>29</v>
       </c>
       <c r="C219" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D219" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F219" t="s">
         <v>255</v>
@@ -4427,10 +4436,10 @@
         <v>221</v>
       </c>
       <c r="C220" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D220" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
@@ -4441,10 +4450,10 @@
         <v>33</v>
       </c>
       <c r="C221" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D221" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
@@ -4455,10 +4464,10 @@
         <v>40</v>
       </c>
       <c r="C222" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D222" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
@@ -4469,10 +4478,10 @@
         <v>170</v>
       </c>
       <c r="C223" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D223" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">
@@ -4483,10 +4492,10 @@
         <v>178</v>
       </c>
       <c r="C224" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D224" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
@@ -4497,10 +4506,10 @@
         <v>257</v>
       </c>
       <c r="C225" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D225" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
@@ -4511,10 +4520,10 @@
         <v>35</v>
       </c>
       <c r="C226" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D226" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
@@ -4525,10 +4534,10 @@
         <v>60</v>
       </c>
       <c r="C227" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D227" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
@@ -4539,10 +4548,10 @@
         <v>141</v>
       </c>
       <c r="C228" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D228" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
@@ -4553,10 +4562,10 @@
         <v>15</v>
       </c>
       <c r="C229" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D229" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
@@ -4567,10 +4576,10 @@
         <v>223</v>
       </c>
       <c r="C230" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D230" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
@@ -4581,10 +4590,10 @@
         <v>9</v>
       </c>
       <c r="C231" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D231" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
@@ -4595,10 +4604,10 @@
         <v>31</v>
       </c>
       <c r="C232" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D232" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
@@ -4609,10 +4618,10 @@
         <v>11</v>
       </c>
       <c r="C233" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D233" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
@@ -4623,10 +4632,10 @@
         <v>13</v>
       </c>
       <c r="C234" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D234" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
@@ -4637,10 +4646,10 @@
         <v>6</v>
       </c>
       <c r="C235" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D235" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
@@ -4651,10 +4660,10 @@
         <v>63</v>
       </c>
       <c r="C236" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D236" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
@@ -4665,10 +4674,10 @@
         <v>17</v>
       </c>
       <c r="C237" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D237" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
@@ -4679,10 +4688,10 @@
         <v>42</v>
       </c>
       <c r="C238" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D238" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
@@ -4693,10 +4702,10 @@
         <v>143</v>
       </c>
       <c r="C239" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D239" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
@@ -4707,10 +4716,10 @@
         <v>161</v>
       </c>
       <c r="C240" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D240" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.2">
@@ -4721,10 +4730,10 @@
         <v>245</v>
       </c>
       <c r="C241" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D241" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.2">
@@ -4735,10 +4744,10 @@
         <v>47</v>
       </c>
       <c r="C242" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D242" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.2">
@@ -4749,10 +4758,10 @@
         <v>52</v>
       </c>
       <c r="C243" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D243" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.2">
@@ -4763,10 +4772,10 @@
         <v>246</v>
       </c>
       <c r="C244" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D244" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.2">
@@ -4777,10 +4786,10 @@
         <v>37</v>
       </c>
       <c r="C245" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D245" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.2">
@@ -4791,10 +4800,10 @@
         <v>176</v>
       </c>
       <c r="C246" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D246" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.2">
@@ -4805,10 +4814,10 @@
         <v>23</v>
       </c>
       <c r="C247" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D247" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.2">
@@ -4819,10 +4828,10 @@
         <v>19</v>
       </c>
       <c r="C248" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D248" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.2">
@@ -4833,10 +4842,10 @@
         <v>215</v>
       </c>
       <c r="C249" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D249" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.2">
@@ -4847,10 +4856,10 @@
         <v>25</v>
       </c>
       <c r="C250" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D250" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.2">
@@ -4861,10 +4870,10 @@
         <v>254</v>
       </c>
       <c r="C251" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D251" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.2">
@@ -4875,24 +4884,24 @@
         <v>261</v>
       </c>
       <c r="C252" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D252" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B253" t="s">
         <v>262</v>
       </c>
       <c r="C253" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D253" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.2">
@@ -4903,10 +4912,10 @@
         <v>260</v>
       </c>
       <c r="C254" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D254" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.2">
@@ -4917,10 +4926,10 @@
         <v>29</v>
       </c>
       <c r="C255" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D255" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F255" t="s">
         <v>263</v>
@@ -4934,10 +4943,10 @@
         <v>221</v>
       </c>
       <c r="C256" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D256" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
@@ -4948,10 +4957,10 @@
         <v>33</v>
       </c>
       <c r="C257" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D257" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
@@ -4962,10 +4971,10 @@
         <v>40</v>
       </c>
       <c r="C258" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D258" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
@@ -4976,10 +4985,10 @@
         <v>170</v>
       </c>
       <c r="C259" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D259" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
@@ -4990,10 +4999,10 @@
         <v>178</v>
       </c>
       <c r="C260" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D260" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
@@ -5004,10 +5013,10 @@
         <v>257</v>
       </c>
       <c r="C261" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D261" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
@@ -5018,10 +5027,10 @@
         <v>35</v>
       </c>
       <c r="C262" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D262" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
@@ -5032,10 +5041,10 @@
         <v>60</v>
       </c>
       <c r="C263" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D263" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
@@ -5046,10 +5055,10 @@
         <v>141</v>
       </c>
       <c r="C264" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D264" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
@@ -5060,10 +5069,10 @@
         <v>15</v>
       </c>
       <c r="C265" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D265" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
@@ -5074,10 +5083,10 @@
         <v>223</v>
       </c>
       <c r="C266" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D266" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
@@ -5088,10 +5097,10 @@
         <v>9</v>
       </c>
       <c r="C267" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D267" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
@@ -5102,10 +5111,10 @@
         <v>31</v>
       </c>
       <c r="C268" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D268" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
@@ -5116,10 +5125,10 @@
         <v>11</v>
       </c>
       <c r="C269" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D269" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
@@ -5130,10 +5139,10 @@
         <v>13</v>
       </c>
       <c r="C270" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D270" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
@@ -5144,10 +5153,10 @@
         <v>6</v>
       </c>
       <c r="C271" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D271" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
@@ -5158,10 +5167,10 @@
         <v>63</v>
       </c>
       <c r="C272" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D272" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
@@ -5172,10 +5181,10 @@
         <v>17</v>
       </c>
       <c r="C273" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D273" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
@@ -5186,10 +5195,10 @@
         <v>42</v>
       </c>
       <c r="C274" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D274" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
@@ -5200,10 +5209,10 @@
         <v>143</v>
       </c>
       <c r="C275" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D275" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
@@ -5214,10 +5223,10 @@
         <v>161</v>
       </c>
       <c r="C276" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D276" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
@@ -5228,10 +5237,10 @@
         <v>245</v>
       </c>
       <c r="C277" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D277" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
@@ -5242,10 +5251,10 @@
         <v>47</v>
       </c>
       <c r="C278" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D278" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
@@ -5256,10 +5265,10 @@
         <v>52</v>
       </c>
       <c r="C279" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D279" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
@@ -5270,10 +5279,10 @@
         <v>246</v>
       </c>
       <c r="C280" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D280" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
@@ -5284,10 +5293,10 @@
         <v>37</v>
       </c>
       <c r="C281" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D281" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
@@ -5298,10 +5307,10 @@
         <v>176</v>
       </c>
       <c r="C282" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D282" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
@@ -5312,10 +5321,10 @@
         <v>23</v>
       </c>
       <c r="C283" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D283" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
@@ -5326,10 +5335,10 @@
         <v>19</v>
       </c>
       <c r="C284" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D284" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
@@ -5340,10 +5349,10 @@
         <v>215</v>
       </c>
       <c r="C285" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D285" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.2">
@@ -5354,10 +5363,10 @@
         <v>25</v>
       </c>
       <c r="C286" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D286" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.2">
@@ -5368,10 +5377,10 @@
         <v>254</v>
       </c>
       <c r="C287" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D287" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.2">
@@ -5382,24 +5391,24 @@
         <v>261</v>
       </c>
       <c r="C288" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D288" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B289" t="s">
         <v>262</v>
       </c>
       <c r="C289" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D289" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.2">
@@ -5410,10 +5419,10 @@
         <v>260</v>
       </c>
       <c r="C290" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D290" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.2">
@@ -5427,7 +5436,7 @@
         <v>7</v>
       </c>
       <c r="D291" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F291" t="s">
         <v>208</v>
@@ -5444,7 +5453,7 @@
         <v>7</v>
       </c>
       <c r="D292" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.2">
@@ -5458,7 +5467,7 @@
         <v>7</v>
       </c>
       <c r="D293" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.2">
@@ -5472,7 +5481,7 @@
         <v>7</v>
       </c>
       <c r="D294" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.2">
@@ -5486,7 +5495,7 @@
         <v>7</v>
       </c>
       <c r="D295" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.2">
@@ -5500,7 +5509,7 @@
         <v>7</v>
       </c>
       <c r="D296" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.2">
@@ -5514,7 +5523,7 @@
         <v>7</v>
       </c>
       <c r="D297" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.2">
@@ -5528,7 +5537,7 @@
         <v>7</v>
       </c>
       <c r="D298" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.2">
@@ -5542,7 +5551,7 @@
         <v>7</v>
       </c>
       <c r="D299" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.2">
@@ -5556,7 +5565,7 @@
         <v>7</v>
       </c>
       <c r="D300" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.2">
@@ -5570,7 +5579,7 @@
         <v>7</v>
       </c>
       <c r="D301" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.2">
@@ -5584,7 +5593,7 @@
         <v>7</v>
       </c>
       <c r="D302" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.2">
@@ -5598,7 +5607,7 @@
         <v>7</v>
       </c>
       <c r="D303" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.2">
@@ -5612,7 +5621,7 @@
         <v>7</v>
       </c>
       <c r="D304" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.2">
@@ -5626,7 +5635,7 @@
         <v>7</v>
       </c>
       <c r="D305" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.2">
@@ -5682,7 +5691,7 @@
         <v>43</v>
       </c>
       <c r="D309" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F309" t="s">
         <v>209</v>
@@ -5699,7 +5708,7 @@
         <v>43</v>
       </c>
       <c r="D310" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.2">
@@ -5713,7 +5722,7 @@
         <v>43</v>
       </c>
       <c r="D311" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.2">
@@ -5727,7 +5736,7 @@
         <v>43</v>
       </c>
       <c r="D312" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.2">
@@ -5741,7 +5750,7 @@
         <v>43</v>
       </c>
       <c r="D313" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.2">
@@ -5755,7 +5764,7 @@
         <v>43</v>
       </c>
       <c r="D314" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.2">
@@ -5769,7 +5778,7 @@
         <v>43</v>
       </c>
       <c r="D315" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.2">
@@ -5783,7 +5792,7 @@
         <v>43</v>
       </c>
       <c r="D316" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.2">
@@ -5797,7 +5806,7 @@
         <v>43</v>
       </c>
       <c r="D317" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.2">
@@ -5811,7 +5820,7 @@
         <v>43</v>
       </c>
       <c r="D318" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.2">
@@ -5825,7 +5834,7 @@
         <v>43</v>
       </c>
       <c r="D319" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.2">
@@ -5839,7 +5848,7 @@
         <v>43</v>
       </c>
       <c r="D320" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.2">
@@ -5853,7 +5862,7 @@
         <v>43</v>
       </c>
       <c r="D321" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.2">
@@ -5867,7 +5876,7 @@
         <v>43</v>
       </c>
       <c r="D322" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.2">
@@ -5881,7 +5890,7 @@
         <v>43</v>
       </c>
       <c r="D323" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.2">
@@ -6593,7 +6602,7 @@
         <v>126</v>
       </c>
       <c r="D370" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F370" t="s">
         <v>210</v>
@@ -6610,7 +6619,7 @@
         <v>126</v>
       </c>
       <c r="D371" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="372" spans="1:6" x14ac:dyDescent="0.2">
@@ -6624,7 +6633,7 @@
         <v>126</v>
       </c>
       <c r="D372" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="373" spans="1:6" x14ac:dyDescent="0.2">
@@ -6638,7 +6647,7 @@
         <v>126</v>
       </c>
       <c r="D373" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="374" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -6652,7 +6661,7 @@
         <v>126</v>
       </c>
       <c r="D374" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E374"/>
       <c r="F374"/>
@@ -6668,7 +6677,7 @@
         <v>126</v>
       </c>
       <c r="D375" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="376" spans="1:6" x14ac:dyDescent="0.2">
@@ -6682,7 +6691,7 @@
         <v>126</v>
       </c>
       <c r="D376" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="377" spans="1:6" x14ac:dyDescent="0.2">
@@ -6696,7 +6705,7 @@
         <v>126</v>
       </c>
       <c r="D377" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="378" spans="1:6" x14ac:dyDescent="0.2">
@@ -6710,7 +6719,7 @@
         <v>126</v>
       </c>
       <c r="D378" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="379" spans="1:6" x14ac:dyDescent="0.2">
@@ -6724,7 +6733,7 @@
         <v>126</v>
       </c>
       <c r="D379" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="380" spans="1:6" x14ac:dyDescent="0.2">
@@ -6738,7 +6747,7 @@
         <v>126</v>
       </c>
       <c r="D380" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="381" spans="1:6" x14ac:dyDescent="0.2">
@@ -6752,7 +6761,7 @@
         <v>126</v>
       </c>
       <c r="D381" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="382" spans="1:6" x14ac:dyDescent="0.2">
@@ -6766,7 +6775,7 @@
         <v>126</v>
       </c>
       <c r="D382" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="383" spans="1:6" x14ac:dyDescent="0.2">
@@ -6777,7 +6786,7 @@
         <v>126</v>
       </c>
       <c r="D383" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E383" t="s">
         <v>128</v>
@@ -6794,7 +6803,7 @@
         <v>126</v>
       </c>
       <c r="D384" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.2">
@@ -6808,7 +6817,7 @@
         <v>126</v>
       </c>
       <c r="D385" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.2">
@@ -6822,7 +6831,7 @@
         <v>126</v>
       </c>
       <c r="D386" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.2">
@@ -6836,7 +6845,7 @@
         <v>126</v>
       </c>
       <c r="D387" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.2">
@@ -6850,7 +6859,7 @@
         <v>126</v>
       </c>
       <c r="D388" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.2">
@@ -6864,7 +6873,7 @@
         <v>126</v>
       </c>
       <c r="D389" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.2">
@@ -6878,7 +6887,7 @@
         <v>126</v>
       </c>
       <c r="D390" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.2">
@@ -7777,7 +7786,7 @@
         <v>186</v>
       </c>
       <c r="D443" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F443" t="s">
         <v>211</v>
@@ -7794,7 +7803,7 @@
         <v>186</v>
       </c>
       <c r="D444" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="445" spans="1:6" x14ac:dyDescent="0.2">
@@ -7808,7 +7817,7 @@
         <v>186</v>
       </c>
       <c r="D445" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="446" spans="1:6" x14ac:dyDescent="0.2">
@@ -7822,7 +7831,7 @@
         <v>186</v>
       </c>
       <c r="D446" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="447" spans="1:6" x14ac:dyDescent="0.2">
@@ -7836,7 +7845,7 @@
         <v>186</v>
       </c>
       <c r="D447" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="448" spans="1:6" x14ac:dyDescent="0.2">
@@ -7850,7 +7859,7 @@
         <v>186</v>
       </c>
       <c r="D448" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.2">
@@ -7864,7 +7873,7 @@
         <v>186</v>
       </c>
       <c r="D449" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.2">
@@ -7878,7 +7887,7 @@
         <v>186</v>
       </c>
       <c r="D450" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.2">
@@ -7892,7 +7901,7 @@
         <v>186</v>
       </c>
       <c r="D451" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.2">
@@ -7906,7 +7915,7 @@
         <v>186</v>
       </c>
       <c r="D452" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.2">
@@ -7920,7 +7929,7 @@
         <v>186</v>
       </c>
       <c r="D453" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.2">
@@ -7934,7 +7943,7 @@
         <v>186</v>
       </c>
       <c r="D454" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.2">
@@ -7948,7 +7957,7 @@
         <v>186</v>
       </c>
       <c r="D455" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.2">
@@ -7962,7 +7971,7 @@
         <v>186</v>
       </c>
       <c r="D456" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.2">
@@ -7976,7 +7985,7 @@
         <v>186</v>
       </c>
       <c r="D457" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.2">
@@ -7990,7 +7999,7 @@
         <v>186</v>
       </c>
       <c r="D458" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.2">
@@ -8004,7 +8013,7 @@
         <v>186</v>
       </c>
       <c r="D459" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.2">
@@ -8018,7 +8027,7 @@
         <v>186</v>
       </c>
       <c r="D460" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.2">
@@ -8032,7 +8041,7 @@
         <v>186</v>
       </c>
       <c r="D461" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.2">
@@ -8046,7 +8055,7 @@
         <v>186</v>
       </c>
       <c r="D462" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.2">
@@ -8060,7 +8069,7 @@
         <v>186</v>
       </c>
       <c r="D463" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.2">
@@ -8074,7 +8083,7 @@
         <v>186</v>
       </c>
       <c r="D464" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="465" spans="1:5" x14ac:dyDescent="0.2">
@@ -9312,15 +9321,15 @@
         <v>207</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C2" s="2">
         <v>24567</v>
@@ -9335,10 +9344,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C3" s="2">
         <v>26120</v>
@@ -9353,10 +9362,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C4" s="2">
         <v>26520</v>
@@ -9374,7 +9383,7 @@
         <v>229</v>
       </c>
       <c r="B5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C5" s="2">
         <v>26795</v>
@@ -9389,10 +9398,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C6" s="2">
         <v>28478</v>
@@ -9407,10 +9416,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C7" s="2">
         <v>29840</v>
@@ -9425,10 +9434,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C8" s="2">
         <v>30100</v>
@@ -9446,7 +9455,7 @@
         <v>232</v>
       </c>
       <c r="B9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C9" s="2">
         <v>30259</v>
@@ -9461,10 +9470,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C10" s="2">
         <v>31607</v>
@@ -9479,10 +9488,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C11" s="2">
         <v>32819</v>
@@ -9497,10 +9506,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C12" s="2">
         <v>34568</v>
@@ -9518,7 +9527,7 @@
         <v>250</v>
       </c>
       <c r="B13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C13" s="2">
         <v>36010</v>
@@ -9533,10 +9542,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C14" s="2">
         <v>37429</v>
@@ -9551,10 +9560,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C15" s="2">
         <v>37768</v>
@@ -9569,10 +9578,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C16" s="2">
         <v>38905</v>
@@ -9587,10 +9596,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C17" s="2">
         <v>39135</v>
@@ -9608,7 +9617,7 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C18" s="2">
         <v>40465</v>
@@ -9626,7 +9635,7 @@
         <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C19" s="2">
         <v>41218</v>
@@ -9644,7 +9653,7 @@
         <v>126</v>
       </c>
       <c r="B20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C20" s="2">
         <v>43034</v>
@@ -9662,18 +9671,18 @@
         <v>186</v>
       </c>
       <c r="B21" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C21" s="2">
         <v>44571</v>
       </c>
       <c r="D21" s="5">
         <f ca="1">NOW()</f>
-        <v>45188.508756249998</v>
+        <v>45314.479231712961</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6904109589041096</v>
+        <v>2.0356164383561643</v>
       </c>
     </row>
   </sheetData>
@@ -9688,6 +9697,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="36475ac5-abd1-4075-8c59-d359717e1992">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9eed236c-863e-4468-81ea-a1a5634b1ca6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008DD1877411468B4F8815EFA5DFB25A11" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5753e93c23519664160129601ea3ab0c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="36475ac5-abd1-4075-8c59-d359717e1992" xmlns:ns3="9eed236c-863e-4468-81ea-a1a5634b1ca6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3266b339bc74cec8c72749ef8cd9d7e2" ns2:_="" ns3:_="">
     <xsd:import namespace="36475ac5-abd1-4075-8c59-d359717e1992"/>
@@ -9936,27 +9965,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45321A69-3AF3-45A5-BA17-9E1CAB2F6123}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9eed236c-863e-4468-81ea-a1a5634b1ca6"/>
+    <ds:schemaRef ds:uri="36475ac5-abd1-4075-8c59-d359717e1992"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="36475ac5-abd1-4075-8c59-d359717e1992">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9eed236c-863e-4468-81ea-a1a5634b1ca6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A499CA7-670F-4DBE-BC8E-D5862FDEEBC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBE188A7-EE25-449E-B46E-84A22C971FF7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9973,29 +10007,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A499CA7-670F-4DBE-BC8E-D5862FDEEBC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45321A69-3AF3-45A5-BA17-9E1CAB2F6123}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9eed236c-863e-4468-81ea-a1a5634b1ca6"/>
-    <ds:schemaRef ds:uri="36475ac5-abd1-4075-8c59-d359717e1992"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>